<commit_message>
Updates to tables and manuscript
</commit_message>
<xml_diff>
--- a/tables/Table_2.xlsx
+++ b/tables/Table_2.xlsx
@@ -147,6 +147,256 @@
     <t>OPN03</t>
   </si>
   <si>
+    <t>SAL-01</t>
+  </si>
+  <si>
+    <t>47.57 ± 0.83</t>
+  </si>
+  <si>
+    <t>SAL-02</t>
+  </si>
+  <si>
+    <t>45.07 ± 0.84</t>
+  </si>
+  <si>
+    <t>SAL-03</t>
+  </si>
+  <si>
+    <t>44.07 ± 0.82</t>
+  </si>
+  <si>
+    <t>SAL-04</t>
+  </si>
+  <si>
+    <t>47.57 ± 0.84</t>
+  </si>
+  <si>
+    <t>SAL-05</t>
+  </si>
+  <si>
+    <t>48.9 ± 0.77</t>
+  </si>
+  <si>
+    <t>SAL-06</t>
+  </si>
+  <si>
+    <t>44.53 ± 0.74</t>
+  </si>
+  <si>
+    <t>SAL-07</t>
+  </si>
+  <si>
+    <t>47.43 ± 0.96</t>
+  </si>
+  <si>
+    <t>SAL-08</t>
+  </si>
+  <si>
+    <t>47.7 ± 0.9</t>
+  </si>
+  <si>
+    <t>SAL-09</t>
+  </si>
+  <si>
+    <t>44.77 ± 0.8</t>
+  </si>
+  <si>
+    <t>SAL-10</t>
+  </si>
+  <si>
+    <t>43.03 ± 0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIR-11-13 </t>
+  </si>
+  <si>
+    <r>
+      <t>36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cl</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PIR-11-14 </t>
+  </si>
+  <si>
+    <t>47.6 ± 0.83</t>
+  </si>
+  <si>
+    <r>
+      <t>Soum d'Ech</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <t>ECH01</t>
+  </si>
+  <si>
+    <t>42.43 ± 0.98</t>
+  </si>
+  <si>
+    <t>ECH02</t>
+  </si>
+  <si>
+    <r>
+      <t>43.2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <t>ECH03</t>
+  </si>
+  <si>
+    <t>38.86 ± 1.11</t>
+  </si>
+  <si>
+    <t>ECH04</t>
+  </si>
+  <si>
+    <t>38.77 ± 1.05</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Full sample information used for exposure age calculation is provided in the Supplementary Information or is available on GitHub: https://github.com/matt-tomkins/moraine-paper-2020, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Mean of 30 SH R-values ± the Standard Error of the Mean, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> OPN samples from Pallàs et al. (2006), </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> PIR samples from Palacios et al. (2015), </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ECH samples from Rodés (2008), </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Measurement error, see Rodés (2008).  </t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Arànser </t>
     </r>
@@ -157,7 +407,7 @@
         <rFont val="Gill Sans MT"/>
         <family val="2"/>
       </rPr>
-      <t>(Left)</t>
+      <t>(Right)</t>
     </r>
     <r>
       <rPr>
@@ -168,256 +418,6 @@
         <family val="2"/>
       </rPr>
       <t>d</t>
-    </r>
-  </si>
-  <si>
-    <t>SAL-01</t>
-  </si>
-  <si>
-    <t>47.57 ± 0.83</t>
-  </si>
-  <si>
-    <t>SAL-02</t>
-  </si>
-  <si>
-    <t>45.07 ± 0.84</t>
-  </si>
-  <si>
-    <t>SAL-03</t>
-  </si>
-  <si>
-    <t>44.07 ± 0.82</t>
-  </si>
-  <si>
-    <t>SAL-04</t>
-  </si>
-  <si>
-    <t>47.57 ± 0.84</t>
-  </si>
-  <si>
-    <t>SAL-05</t>
-  </si>
-  <si>
-    <t>48.9 ± 0.77</t>
-  </si>
-  <si>
-    <t>SAL-06</t>
-  </si>
-  <si>
-    <t>44.53 ± 0.74</t>
-  </si>
-  <si>
-    <t>SAL-07</t>
-  </si>
-  <si>
-    <t>47.43 ± 0.96</t>
-  </si>
-  <si>
-    <t>SAL-08</t>
-  </si>
-  <si>
-    <t>47.7 ± 0.9</t>
-  </si>
-  <si>
-    <t>SAL-09</t>
-  </si>
-  <si>
-    <t>44.77 ± 0.8</t>
-  </si>
-  <si>
-    <t>SAL-10</t>
-  </si>
-  <si>
-    <t>43.03 ± 0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIR-11-13 </t>
-  </si>
-  <si>
-    <r>
-      <t>36</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Cl</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">PIR-11-14 </t>
-  </si>
-  <si>
-    <t>47.6 ± 0.83</t>
-  </si>
-  <si>
-    <r>
-      <t>Soum d'Ech</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-  </si>
-  <si>
-    <t>ECH01</t>
-  </si>
-  <si>
-    <t>42.43 ± 0.98</t>
-  </si>
-  <si>
-    <t>ECH02</t>
-  </si>
-  <si>
-    <r>
-      <t>43.2</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <t>ECH03</t>
-  </si>
-  <si>
-    <t>38.86 ± 1.11</t>
-  </si>
-  <si>
-    <t>ECH04</t>
-  </si>
-  <si>
-    <t>38.77 ± 1.05</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Full sample information used for exposure age calculation is provided in the Supplementary Information or is available on GitHub: https://github.com/matt-tomkins/moraine-paper-2020, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Mean of 30 SH R-values ± the Standard Error of the Mean, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> OPN samples from Pallàs et al. (2006), </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> PIR samples from Palacios et al. (2015), </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ECH samples from Rodés (2008), </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Measurement error, see Rodés (2008).  </t>
     </r>
   </si>
 </sst>
@@ -535,10 +535,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -851,7 +851,7 @@
   <dimension ref="B2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,7 +914,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -946,7 +946,7 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1006,11 +1006,11 @@
       </c>
     </row>
     <row r="7" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>13</v>
@@ -1034,13 +1034,13 @@
         <v>1.5</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
+      <c r="C8" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -1064,13 +1064,13 @@
         <v>1.5</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>13</v>
@@ -1094,13 +1094,13 @@
         <v>1.7</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="C10" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>13</v>
@@ -1124,13 +1124,13 @@
         <v>1.5</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="6"/>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>13</v>
@@ -1154,13 +1154,13 @@
         <v>1.6</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="6"/>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
@@ -1184,13 +1184,13 @@
         <v>1.5</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="6"/>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>13</v>
@@ -1214,13 +1214,13 @@
         <v>1.4</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
+      <c r="C14" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>13</v>
@@ -1244,13 +1244,13 @@
         <v>1.4</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>13</v>
@@ -1274,13 +1274,13 @@
         <v>1.7</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="7"/>
+      <c r="C16" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
@@ -1304,16 +1304,16 @@
         <v>1.8</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E17" s="2">
         <v>42.421300000000002</v>
@@ -1340,10 +1340,10 @@
     <row r="18" spans="2:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="8"/>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="1">
         <v>42.420900000000003</v>
@@ -1364,15 +1364,15 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="K18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>13</v>
@@ -1396,13 +1396,13 @@
         <v>3.6</v>
       </c>
       <c r="K19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="7"/>
+      <c r="C20" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>13</v>
@@ -1420,7 +1420,7 @@
         <v>59</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="2">
         <v>43</v>
@@ -1430,9 +1430,9 @@
       </c>
     </row>
     <row r="21" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>13</v>
@@ -1456,13 +1456,13 @@
         <v>3.5</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="7"/>
+      <c r="C22" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>13</v>
@@ -1486,12 +1486,12 @@
         <v>3.3</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>

</xml_diff>

<commit_message>
Updates to manuscript based on comments from PH, JH, RP, AR, JA, VR, VJ, LRR, RC, IB and CMD
</commit_message>
<xml_diff>
--- a/tables/Table_2.xlsx
+++ b/tables/Table_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Desktop\Repo\moraine-paper-2020\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BCA393-C46C-412B-89F4-562292D9108B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6DDF76-D031-4B13-8C7B-0A4084A18D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>STD / IQR</t>
   </si>
   <si>
-    <t>3.24 ± 0.68</t>
-  </si>
-  <si>
     <t>1.2 ka</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Right</t>
   </si>
   <si>
-    <t>22.30 ± 0.91</t>
-  </si>
-  <si>
     <t>6.9 ka</t>
   </si>
   <si>
@@ -177,24 +171,15 @@
     <t>Outer</t>
   </si>
   <si>
-    <t>26.20 ± 2.48</t>
-  </si>
-  <si>
     <t>3.5 ka</t>
   </si>
   <si>
     <t>Inner</t>
   </si>
   <si>
-    <t>26.11 ± 1.74</t>
-  </si>
-  <si>
     <t>Combined</t>
   </si>
   <si>
-    <t>27.28 ± 1.78</t>
-  </si>
-  <si>
     <t>3.6 ka</t>
   </si>
   <si>
@@ -244,22 +229,281 @@
   </si>
   <si>
     <r>
-      <t>12.52 ± 0.42</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+      <t>a,b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Method used for kernel density estimation after Silverman (1986) and Dortch </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. (2020) and its associated numeric bandwidth, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">c </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">All model </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> values &lt; 0.01,</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> d </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Reported</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>uncertainty (±) is the 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bounds (68%) of the highest probability component Gaussian, unless stated otherwise, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Interquartile range, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">f </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Shapiro-Wilk test for normality </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> values,</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> g </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Based on the landform age ± 2σ,</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Arithmetic mean of 60 samples ± total uncertainty, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Calculation based on a reduced dataset of 274 samples. Sample ARL-192 (1.97 ± 2.06 ka) is more than three standard deviations from the mean of the remaining samples and was removed for program stability.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 2. </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Gill Sans MT"/>
         <family val="2"/>
       </rPr>
+      <t>Age statistics for the sampled moraines</t>
+    </r>
+  </si>
+  <si>
+    <t>3.2 ± 0.7</t>
+  </si>
+  <si>
+    <r>
+      <t>12.5 ± 0.4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
       <t>h</t>
     </r>
   </si>
   <si>
     <r>
-      <t>23.29 ± 1.12</t>
+      <t>23.3 ± 1.1</t>
     </r>
     <r>
       <rPr>
@@ -273,260 +517,16 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>a,b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Method used for kernel density estimation after Silverman (1986) and Dortch </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>et al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. (2020) and its associated numeric bandwidth, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">c </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">All model </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> values &lt; 0.01,</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> d </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Reported</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>uncertainty (±) is the 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>σ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> bounds (68%) of the highest probability component Gaussian, unless stated otherwise, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Interquartile range, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">f </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Shapiro-Wilk test for normality </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> values,</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> g </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Based on the landform age ± 2σ,</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Arithmetic mean of 60 samples ± total uncertainty, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Calculation based on a reduced dataset of 274 samples. Sample ARL-192 (1.97 ± 2.06 ka) is more than three standard deviations from the mean of the remaining samples and was removed for program stability.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Table 2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Age statistics for the sampled moraines</t>
-    </r>
+    <t>22.3 ± 0.9</t>
+  </si>
+  <si>
+    <t>26.2 ± 2.5</t>
+  </si>
+  <si>
+    <t>26.1 ± 1.7</t>
+  </si>
+  <si>
+    <t>27.3 ± 1.8</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,7 +1019,7 @@
   <sheetData>
     <row r="2" spans="2:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1062,13 +1062,13 @@
         <v>8</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1088,10 +1088,10 @@
         <v>0.99850000000000005</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="I4" s="3">
         <v>0.34</v>
@@ -1111,13 +1111,13 @@
     </row>
     <row r="5" spans="2:13" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="4">
         <v>2.016</v>
@@ -1126,10 +1126,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" s="3">
         <v>-0.24</v>
@@ -1149,13 +1149,13 @@
     </row>
     <row r="6" spans="2:13" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E6" s="5">
         <v>0.70030000000000003</v>
@@ -1164,16 +1164,16 @@
         <v>0.99780000000000002</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="3">
         <v>-1.02</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="8">
         <v>44</v>
@@ -1188,10 +1188,10 @@
     <row r="7" spans="2:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="4">
         <v>0.67959999999999998</v>
@@ -1200,16 +1200,16 @@
         <v>0.99909999999999999</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3">
         <v>-1.1299999999999999</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7" s="8">
         <v>51</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="8" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1238,16 +1238,16 @@
         <v>0.998</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I8" s="3">
         <v>-1.49</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>10</v>
@@ -1262,7 +1262,7 @@
     <row r="9" spans="2:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1274,16 +1274,16 @@
         <v>0.99960000000000004</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I9" s="3">
         <v>-1.05</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>10</v>
@@ -1298,7 +1298,7 @@
     <row r="10" spans="2:13" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -1310,16 +1310,16 @@
         <v>0.99890000000000001</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I10" s="3">
         <v>-1.49</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10" s="8">
         <v>24</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="11" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>

</xml_diff>